<commit_message>
time removed from table
</commit_message>
<xml_diff>
--- a/Backend/RegularCycle.xlsx
+++ b/Backend/RegularCycle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://coepac-my.sharepoint.com/personal/rujutaab21_comp_coeptech_ac_in/Documents/Projects/Hackathon-764/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hackathon-764\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{E34EC0C7-78F2-4D53-A1DB-D278882E739F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41B4301F-3C6A-45B7-8122-5368060440DB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EB9EB1-1218-4704-970C-4CE177349276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="10340" windowHeight="7180" xr2:uid="{FE8E1547-FD77-458A-9196-5BB1C4B232D7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FE8E1547-FD77-458A-9196-5BB1C4B232D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Start</t>
   </si>
@@ -34,6 +34,156 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>2021-01-25</t>
+  </si>
+  <si>
+    <t>2021-01-30</t>
+  </si>
+  <si>
+    <t>2021-02-25</t>
+  </si>
+  <si>
+    <t>2021-03-03</t>
+  </si>
+  <si>
+    <t>2021-03-23</t>
+  </si>
+  <si>
+    <t>2021-03-29</t>
+  </si>
+  <si>
+    <t>2021-04-25</t>
+  </si>
+  <si>
+    <t>2021-05-01</t>
+  </si>
+  <si>
+    <t>2021-05-25</t>
+  </si>
+  <si>
+    <t>2021-05-31</t>
+  </si>
+  <si>
+    <t>2021-06-21</t>
+  </si>
+  <si>
+    <t>2021-06-27</t>
+  </si>
+  <si>
+    <t>2021-07-23</t>
+  </si>
+  <si>
+    <t>2021-07-29</t>
+  </si>
+  <si>
+    <t>2021-08-23</t>
+  </si>
+  <si>
+    <t>2021-08-29</t>
+  </si>
+  <si>
+    <t>2021-09-25</t>
+  </si>
+  <si>
+    <t>2021-09-30</t>
+  </si>
+  <si>
+    <t>2021-10-27</t>
+  </si>
+  <si>
+    <t>2021-11-02</t>
+  </si>
+  <si>
+    <t>2021-11-28</t>
+  </si>
+  <si>
+    <t>2021-12-03</t>
+  </si>
+  <si>
+    <t>2021-12-27</t>
+  </si>
+  <si>
+    <t>2022-01-01</t>
+  </si>
+  <si>
+    <t>2022-01-31</t>
+  </si>
+  <si>
+    <t>2022-02-06</t>
+  </si>
+  <si>
+    <t>2022-03-05</t>
+  </si>
+  <si>
+    <t>2022-03-10</t>
+  </si>
+  <si>
+    <t>2022-04-02</t>
+  </si>
+  <si>
+    <t>2022-04-07</t>
+  </si>
+  <si>
+    <t>2022-05-01</t>
+  </si>
+  <si>
+    <t>2022-05-07</t>
+  </si>
+  <si>
+    <t>2022-06-04</t>
+  </si>
+  <si>
+    <t>2022-06-09</t>
+  </si>
+  <si>
+    <t>2022-07-02</t>
+  </si>
+  <si>
+    <t>2022-07-08</t>
+  </si>
+  <si>
+    <t>2022-07-30</t>
+  </si>
+  <si>
+    <t>2022-08-04</t>
+  </si>
+  <si>
+    <t>2022-08-28</t>
+  </si>
+  <si>
+    <t>2022-09-02</t>
+  </si>
+  <si>
+    <t>2022-09-28</t>
+  </si>
+  <si>
+    <t>2022-10-04</t>
+  </si>
+  <si>
+    <t>2022-10-31</t>
+  </si>
+  <si>
+    <t>2022-11-06</t>
+  </si>
+  <si>
+    <t>2022-12-01</t>
+  </si>
+  <si>
+    <t>2022-12-07</t>
+  </si>
+  <si>
+    <t>2023-01-05</t>
+  </si>
+  <si>
+    <t>2023-01-10</t>
+  </si>
+  <si>
+    <t>2023-02-01</t>
+  </si>
+  <si>
+    <t>2023-02-06</t>
   </si>
 </sst>
 </file>
@@ -395,14 +545,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32021ED-43DD-47D7-9174-9F309909D726}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11.7265625" customWidth="1"/>
     <col min="3" max="3" width="10.7265625" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -420,275 +571,275 @@
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>44221</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44226</v>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>44252</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44258</v>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>44278</v>
-      </c>
-      <c r="C4" s="1">
-        <v>44284</v>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
-        <v>44311</v>
-      </c>
-      <c r="C5" s="1">
-        <v>44317</v>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
-        <v>44341</v>
-      </c>
-      <c r="C6" s="1">
-        <v>44347</v>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
-        <v>44368</v>
-      </c>
-      <c r="C7" s="1">
-        <v>44374</v>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8" s="1">
-        <v>44400</v>
-      </c>
-      <c r="C8" s="1">
-        <v>44406</v>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" s="1">
-        <v>44431</v>
-      </c>
-      <c r="C9" s="1">
-        <v>44437</v>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="1">
-        <v>44464</v>
-      </c>
-      <c r="C10" s="1">
-        <v>44469</v>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2</v>
       </c>
-      <c r="B11" s="1">
-        <v>44496</v>
-      </c>
-      <c r="C11" s="1">
-        <v>44502</v>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2</v>
       </c>
-      <c r="B12" s="1">
-        <v>44528</v>
-      </c>
-      <c r="C12" s="1">
-        <v>44533</v>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" s="1">
-        <v>44557</v>
-      </c>
-      <c r="C13" s="1">
-        <v>44562</v>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2</v>
       </c>
-      <c r="B14" s="1">
-        <v>44592</v>
-      </c>
-      <c r="C14" s="1">
-        <v>44598</v>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
-      <c r="B15" s="1">
-        <v>44625</v>
-      </c>
-      <c r="C15" s="1">
-        <v>44630</v>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="B16" s="1">
-        <v>44653</v>
-      </c>
-      <c r="C16" s="1">
-        <v>44658</v>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
-      <c r="B17" s="1">
-        <v>44682</v>
-      </c>
-      <c r="C17" s="1">
-        <v>44688</v>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="B18" s="1">
-        <v>44716</v>
-      </c>
-      <c r="C18" s="1">
-        <v>44721</v>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
-      <c r="B19" s="1">
-        <v>44744</v>
-      </c>
-      <c r="C19" s="1">
-        <v>44750</v>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2</v>
       </c>
-      <c r="B20" s="1">
-        <v>44772</v>
-      </c>
-      <c r="C20" s="1">
-        <v>44777</v>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2</v>
       </c>
-      <c r="B21" s="1">
-        <v>44801</v>
-      </c>
-      <c r="C21" s="1">
-        <v>44806</v>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
-      <c r="B22" s="1">
-        <v>44832</v>
-      </c>
-      <c r="C22" s="1">
-        <v>44838</v>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2</v>
       </c>
-      <c r="B23" s="1">
-        <v>44865</v>
-      </c>
-      <c r="C23" s="1">
-        <v>44871</v>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2</v>
       </c>
-      <c r="B24" s="1">
-        <v>44896</v>
-      </c>
-      <c r="C24" s="1">
-        <v>44902</v>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2</v>
       </c>
-      <c r="B25" s="1">
-        <v>44931</v>
-      </c>
-      <c r="C25" s="1">
-        <v>44936</v>
+      <c r="B25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2</v>
       </c>
-      <c r="B26" s="1">
-        <v>44958</v>
-      </c>
-      <c r="C26" s="1">
-        <v>44963</v>
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>